<commit_message>
modifications to find optimize base prime load
</commit_message>
<xml_diff>
--- a/logFile_analysis 29052016.xlsx
+++ b/logFile_analysis 29052016.xlsx
@@ -3843,7 +3843,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I2" sqref="I2:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3995,7 +3995,7 @@
         <v>3</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I6" si="3">I5-0.06</f>
+        <f t="shared" ref="I4:I35" si="3">I5-0.06</f>
         <v>0.75999999999999979</v>
       </c>
       <c r="K4">

</xml_diff>